<commit_message>
added pipelined work in main_LQR_realistic.m
</commit_message>
<xml_diff>
--- a/rip/plots/Q_and_R_plots/Set_index_4/param_imp.xlsx
+++ b/rip/plots/Q_and_R_plots/Set_index_4/param_imp.xlsx
@@ -67,7 +67,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -213,6 +213,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>-14.151289456726818</v>
+      </c>
+      <c r="B14" s="0">
+        <v>2.1586155921367434</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>-5.8697131578048243</v>
+      </c>
+      <c r="B15" s="0">
+        <v>3.6195920279994089</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>-2.1586155921367434</v>
+      </c>
+      <c r="B16" s="0">
+        <v>5.8697131578048243</v>
+      </c>
+      <c r="C16" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>-3.6195920279994089</v>
+      </c>
+      <c r="B17" s="0">
+        <v>14.151289456726818</v>
+      </c>
+      <c r="C17" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compiled slx to 2021b
</commit_message>
<xml_diff>
--- a/rip/plots/Q_and_R_plots/Set_index_4/param_imp.xlsx
+++ b/rip/plots/Q_and_R_plots/Set_index_4/param_imp.xlsx
@@ -42,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -51,13 +51,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -67,7 +69,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -257,6 +259,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>-14.151289456726818</v>
+      </c>
+      <c r="B18" s="0">
+        <v>2.1586155921367434</v>
+      </c>
+      <c r="C18" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>-5.8697131578048243</v>
+      </c>
+      <c r="B19" s="0">
+        <v>3.6195920279994089</v>
+      </c>
+      <c r="C19" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>-2.1586155921367434</v>
+      </c>
+      <c r="B20" s="0">
+        <v>5.8697131578048243</v>
+      </c>
+      <c r="C20" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>-3.6195920279994089</v>
+      </c>
+      <c r="B21" s="0">
+        <v>14.151289456726818</v>
+      </c>
+      <c r="C21" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>